<commit_message>
Adding Traffic Distribution Case Excel
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C49988
</commit_message>
<xml_diff>
--- a/TOneV2/Documents/Routing/Traffic Distribution Case.xlsx
+++ b/TOneV2/Documents/Routing/Traffic Distribution Case.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,102 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Option 3</t>
+  </si>
+  <si>
+    <t>Option 4</t>
+  </si>
+  <si>
+    <t>Option 5</t>
+  </si>
+  <si>
+    <t>CAN BE ALTERED</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Reversed Rate</t>
+  </si>
+  <si>
+    <t>normalized Services</t>
+  </si>
+  <si>
+    <t>normalized Quality</t>
+  </si>
+  <si>
+    <t>normalized Rate</t>
+  </si>
+  <si>
+    <t>Factors:</t>
+  </si>
+  <si>
+    <t>Quality Traffic Percentage</t>
+  </si>
+  <si>
+    <t>Rate Traffic Percentage</t>
+  </si>
+  <si>
+    <t>Services Traffic Percentage</t>
+  </si>
+  <si>
+    <t>Total Traffic Percentages</t>
+  </si>
+  <si>
+    <t>Not Blocked</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>We are going to take the best 3 options, so  we will take 1, 2 and 3 since 4 is blocked. This will make the best rate be removed.</t>
+  </si>
+  <si>
+    <t>But if we have removed option 4 from the start, a drastic change in option 5 new percentage would be 54% even higher to what option 4 was!</t>
+  </si>
+  <si>
+    <t>This means that our current system will leave option 5 behind even though it’s a great option when option 4 is removed.</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +112,74 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -40,19 +187,324 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Curved Right Arrow 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="2438400"/>
+          <a:ext cx="828675" cy="1666875"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedRightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table2" ref="C1:H15" totalsRowCount="1">
+  <autoFilter ref="C1:H14"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Column1" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="Option 1" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Option 2" totalsRowDxfId="3"/>
+    <tableColumn id="4" name="Option 3" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Option 4" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Option 5" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table3" ref="C20:H33" totalsRowShown="0">
+  <autoFilter ref="C20:H33"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Option 1"/>
+    <tableColumn id="3" name="Option 2"/>
+    <tableColumn id="4" name="Option 3"/>
+    <tableColumn id="5" name="Option 4"/>
+    <tableColumn id="6" name="Option 5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -98,7 +550,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +585,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +793,688 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>355</v>
+      </c>
+      <c r="E3" s="1">
+        <v>450</v>
+      </c>
+      <c r="F3" s="1">
+        <v>400</v>
+      </c>
+      <c r="G3" s="1">
+        <v>200</v>
+      </c>
+      <c r="H3" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:H6" si="0">POWER(D5,-1)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <f>D4/MAX(4:4)</f>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>E4/MAX(4:4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <f>F4/MAX(4:4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <f>G4/MAX(4:4)</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H7">
+        <f>H4/MAX(4:4)</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <f>D3/MAX(3:3)</f>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="E8">
+        <f>E3/MAX(3:3)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F8">
+        <f>F3/MAX(3:3)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G8">
+        <f>G3/MAX(3:3)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H8">
+        <f>H3/MAX(3:3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <f>D6/MAX(6:6)</f>
+        <v>3.3333333333333333E-6</v>
+      </c>
+      <c r="E9">
+        <f>E6/MAX(6:6)</f>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="F9">
+        <f>F6/MAX(6:6)</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G9">
+        <f>G6/MAX(6:6)</f>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>H6/MAX(6:6)</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <f>D8*$B10/(SUM(8:8))</f>
+        <v>3.5411471321695762</v>
+      </c>
+      <c r="E10">
+        <f>E8*$B10/(SUM(8:8))</f>
+        <v>4.4887780548628431</v>
+      </c>
+      <c r="F10">
+        <f>F8*$B10/(SUM(8:8))</f>
+        <v>3.9900249376558596</v>
+      </c>
+      <c r="G10">
+        <f>G8*$B10/(SUM(8:8))</f>
+        <v>1.9950124688279298</v>
+      </c>
+      <c r="H10">
+        <f>(H8*$B10)/(SUM(8:8))</f>
+        <v>5.9850374064837899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <f>D9*$B11/(SUM(9:9))</f>
+        <v>1.6649711710241741E-4</v>
+      </c>
+      <c r="E11">
+        <f>E9*$B11/(SUM(9:9))</f>
+        <v>2.4974567565362609E-4</v>
+      </c>
+      <c r="F11">
+        <f>F9*$B11/(SUM(9:9))</f>
+        <v>4.9949135130725219E-4</v>
+      </c>
+      <c r="G11">
+        <f>G9*$B11/(SUM(9:9))</f>
+        <v>49.949135130725224</v>
+      </c>
+      <c r="H11">
+        <f>H9*$B11/(SUM(9:9))</f>
+        <v>4.9949135130725228E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <f>D7*$B12/(SUM(7:7))</f>
+        <v>14.354066985645934</v>
+      </c>
+      <c r="E12">
+        <f>E7*$B12/(SUM(7:7))</f>
+        <v>7.1770334928229671</v>
+      </c>
+      <c r="F12">
+        <f>F7*$B12/(SUM(7:7))</f>
+        <v>7.1770334928229671</v>
+      </c>
+      <c r="G12">
+        <f>G7*$B12/(SUM(7:7))</f>
+        <v>0.64593301435406691</v>
+      </c>
+      <c r="H12">
+        <f>H7*$B12/(SUM(7:7))</f>
+        <v>0.64593301435406691</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <f>D10+D11+D12</f>
+        <v>17.895380614932613</v>
+      </c>
+      <c r="E13">
+        <f>E10+E11+E12</f>
+        <v>11.666061293361464</v>
+      </c>
+      <c r="F13">
+        <f>F10+F11+F12</f>
+        <v>11.167557921830134</v>
+      </c>
+      <c r="G13" s="5">
+        <f>G10+G11+G12</f>
+        <v>52.590080613907219</v>
+      </c>
+      <c r="H13" s="5">
+        <f>H10+H11+H12</f>
+        <v>6.6809195559685817</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="6"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J19" s="21"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="22"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>355</v>
+      </c>
+      <c r="E23" s="1">
+        <v>450</v>
+      </c>
+      <c r="F23" s="1">
+        <v>400</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1">
+        <v>20</v>
+      </c>
+      <c r="E24" s="1">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:H26" si="1">POWER(D25,-1)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <f>D24/MAX(24:24)</f>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f>E24/MAX(24:24)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F27">
+        <f>F24/MAX(24:24)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H27">
+        <f>H24/MAX(24:24)</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <f>D23/MAX(23:23)</f>
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="E28">
+        <f>E23/MAX(23:23)</f>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f>F23/MAX(23:23)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="H28">
+        <f>H23/MAX(23:23)</f>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <f>D26/MAX(26:26)</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="E29">
+        <f>E26/MAX(26:26)</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F29">
+        <f>F26/MAX(26:26)</f>
+        <v>0.01</v>
+      </c>
+      <c r="H29">
+        <f>H26/MAX(26:26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="1">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <f>D28*$B30/(SUM(28:28))</f>
+        <v>4.565916398713826</v>
+      </c>
+      <c r="E30">
+        <f>E28*$B30/(SUM(28:28))</f>
+        <v>5.7877813504823159</v>
+      </c>
+      <c r="F30">
+        <f>F28*$B30/(SUM(28:28))</f>
+        <v>5.1446945337620589</v>
+      </c>
+      <c r="H30">
+        <f>(H28*$B30)/(SUM(28:28))</f>
+        <v>4.501607717041801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <f>D29*$B31/(SUM(29:29))</f>
+        <v>0.16366612111292964</v>
+      </c>
+      <c r="E31">
+        <f>E29*$B31/(SUM(29:29))</f>
+        <v>0.24549918166939444</v>
+      </c>
+      <c r="F31">
+        <f>F29*$B31/(SUM(29:29))</f>
+        <v>0.49099836333878888</v>
+      </c>
+      <c r="H31">
+        <f>H29*$B31/(SUM(29:29))</f>
+        <v>49.099836333878891</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <f>D27*$B32/(SUM(27:27))</f>
+        <v>14.669926650366749</v>
+      </c>
+      <c r="E32">
+        <f>E27*$B32/(SUM(27:27))</f>
+        <v>7.3349633251833746</v>
+      </c>
+      <c r="F32">
+        <f>F27*$B32/(SUM(27:27))</f>
+        <v>7.3349633251833746</v>
+      </c>
+      <c r="H32">
+        <f>H27*$B32/(SUM(27:27))</f>
+        <v>0.6601466992665036</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33">
+        <f>D30+D31+D32</f>
+        <v>19.399509170193504</v>
+      </c>
+      <c r="E33">
+        <f>E30+E31+E32</f>
+        <v>13.368243857335084</v>
+      </c>
+      <c r="F33">
+        <f>F30+F31+F32</f>
+        <v>12.970656222284223</v>
+      </c>
+      <c r="H33" s="5">
+        <f>H30+H31+H32</f>
+        <v>54.261590750187196</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>